<commit_message>
Changed the column widths to 16 in the Payments sheet. Centered and text wrapped the column heddings.
</commit_message>
<xml_diff>
--- a/AyanaScottElliston_Week2Homework 1.xlsx
+++ b/AyanaScottElliston_Week2Homework 1.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28706"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC7A1B7C-3715-4B46-955F-7198649EE0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79252E75-9DC0-43EB-8288-0E6B393048B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="9115" r:id="rId5"/>
+    <pivotCache cacheId="82" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -716,7 +716,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
@@ -725,12 +724,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -741,6 +743,15 @@
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
@@ -748,6 +759,21 @@
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -983,6 +1009,62 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -6599,7 +6681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1597348B-385D-40FD-BC76-CCEBE441CE4F}" name="PivotTable1" cacheId="9115" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1597348B-385D-40FD-BC76-CCEBE441CE4F}" name="PivotTable1" cacheId="82" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
@@ -6815,7 +6897,7 @@
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <formats count="8">
+  <formats count="16">
     <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
@@ -6826,22 +6908,82 @@
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="3">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
+    <format dxfId="13">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    <format dxfId="14">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    <format dxfId="15">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="3">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -6871,6 +7013,18 @@
           </reference>
           <reference field="6" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -7198,8 +7352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13286,261 +13440,259 @@
   <dimension ref="A3:E275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="25" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" s="28" customFormat="1">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:5" s="27" customFormat="1" ht="30.75">
+      <c r="A3" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
-      <c r="E3"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="28" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>40910</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>1000</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>40913</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="25">
         <v>340</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25">
         <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>40923</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="25">
         <v>80</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>35</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>40924</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="25">
         <v>1392</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="25">
         <v>105</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="25">
         <v>1497</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="25">
+      <c r="A9" s="24">
         <v>40928</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="25">
         <v>20000</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>-20000</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26">
+      <c r="D9" s="25"/>
+      <c r="E9" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="25">
+      <c r="A10" s="24">
         <v>40929</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="D10" s="26">
+      <c r="B10" s="25"/>
+      <c r="D10" s="25">
         <v>61</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="25">
+      <c r="A11" s="24">
         <v>40934</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>6720</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>20000</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25">
         <v>26720</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="25">
+      <c r="A12" s="24">
         <v>40939</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>738.25</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="25">
         <v>-170</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="25">
         <v>568.25</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="25">
+      <c r="A13" s="24">
         <v>40941</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>1000</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25">
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="25">
+      <c r="A14" s="24">
         <v>40944</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>340</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26">
+      <c r="D14" s="25"/>
+      <c r="E14" s="25">
         <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="25">
+      <c r="A15" s="24">
         <v>40954</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="25">
         <v>80</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="25">
         <v>35</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25">
         <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="25">
+      <c r="A16" s="24">
         <v>40959</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="25">
         <v>20000</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="25">
         <v>-20000</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26">
+      <c r="D16" s="25"/>
+      <c r="E16" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="25">
+      <c r="A17" s="24">
         <v>40964</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="25">
         <v>2200</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="25">
         <v>75</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="25">
         <v>2275</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="25">
+      <c r="A18" s="24">
         <v>40965</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="25">
         <v>6720</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="25">
         <v>20000</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26">
+      <c r="D18" s="25"/>
+      <c r="E18" s="25">
         <v>26720</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="25">
+      <c r="A19" s="24">
         <v>40966</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="25">
         <v>514</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26">
+      <c r="D19" s="25"/>
+      <c r="E19" s="25">
         <v>514</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="25">
+      <c r="A20" s="24">
         <v>40968</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <v>3770</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="25">
         <v>-70</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="25">
         <v>3700</v>
       </c>
     </row>
@@ -13548,16 +13700,16 @@
       <c r="A21" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="25">
         <v>64894.25</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="25">
         <v>70</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="25">
         <v>1</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="25">
         <v>64965.25</v>
       </c>
     </row>
@@ -14602,7 +14754,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" activeCellId="2" sqref="A4:A8 G4:G8 B4:B8"/>
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>